<commit_message>
Update compte utilisateurs PB Boolean Update Looping pour implémentation DB
</commit_message>
<xml_diff>
--- a/docs/Compte utilisateurs.xlsx
+++ b/docs/Compte utilisateurs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CDA-11\Desktop\Projet\JDR2D\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CDA-11\Desktop\Projet\jdr2d\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683D2FE1-770F-45DF-9F5B-F6EA3EFC8CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F1B990-E84F-4492-9D81-1C18695D2EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9BD0C550-A797-4853-952F-535C25738A5C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9BD0C550-A797-4853-952F-535C25738A5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -465,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -476,9 +476,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -488,71 +485,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -936,7 +930,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F7" sqref="F7:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,182 +972,182 @@
       <c r="H1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16" t="s">
+      <c r="E2" s="9"/>
+      <c r="F2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="25" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="10"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="26"/>
     </row>
     <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="10"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="26"/>
     </row>
     <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5" t="s">
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="10"/>
+      <c r="J5" s="26"/>
       <c r="L5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="7" t="s">
+      <c r="G6" s="4"/>
+      <c r="H6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="6">
         <v>4</v>
       </c>
-      <c r="J6" s="10"/>
+      <c r="J6" s="26"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="8" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="9">
+      <c r="F7" s="18"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="23">
         <v>5</v>
       </c>
-      <c r="J7" s="10"/>
+      <c r="J7" s="26"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="26"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="14"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="27"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
@@ -1400,13 +1394,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="J2:J8"/>
     <mergeCell ref="A7:C8"/>
     <mergeCell ref="F7:H8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="I2:I4"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J2:J8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>